<commit_message>
🔄 Update extracted and deduplicated ambassador application data
</commit_message>
<xml_diff>
--- a/ambassador/submissions_duplicates_removed.xlsx
+++ b/ambassador/submissions_duplicates_removed.xlsx
@@ -469,10 +469,26 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>🏆 Ambassador Contribution Plan:
-🔗 Additional Information:
-✅ Contribution Highlights:
-I am **nominating someone else** to become a PyTorch Ambassador.; The nominee is **18 years of age or older**.; The nominee **agrees to abide by the [PyTorch Code of Conduct](https://github.com/pytorch-fdn/Foundation/blob/main/PyTorch%20Foundation%20Code%20of%20Conduct.md)**.; The nominee **agrees to comply with the [Linux Foundation Antitrust Policy](https://www.linuxfoundation.org/legal/antitrust-policy)**.; The nominee meets **at least one** of the qualifications listed in the [PyTorch Ambassador Program Requirements](https://github.com/pytorch-fdn/ambassador-program/blob/main/README.md).; An active leader in the PyTorch community with **at least one year** of experience in:; Organizing events (virtual/in-person).; Speaking at AI/ML conferences.; Mentoring others in PyTorch.</t>
+          <t>Contributions:
+- [ ] I am **nominating myself** for the PyTorch Ambassador Program.
+- [x] I am **nominating someone else** to become a PyTorch Ambassador.
+- [x] The nominee is **18 years of age or older**.
+- [x] The nominee **agrees to abide by the [PyTorch Code of Conduct](https://github.com/pytorch-fdn/Foundation/blob/main/PyTorch%20Foundation%20Code%20of%20Conduct.md)**.
+- [x] The nominee **agrees to comply with the [Linux Foundation Antitrust Policy](https://www.linuxfoundation.org/legal/antitrust-policy)**.
+- [x] The nominee meets **at least one** of the qualifications listed in the [PyTorch Ambassador Program Requirements](https://github.com/pytorch-fdn/ambassador-program/blob/main/README.md).
+- [ ] An active contributor to PyTorch repositories (e.g., commits, PRs, discussions).
+- [ ] A speaker at PyTorch events or workshops.
+- [ ] A PyTorch user group organizer or meetup host.
+- [ ] A researcher or educator using PyTorch in academic work or training.
+- [x] An active leader in the PyTorch community with **at least one year** of experience in:
+- [x] Organizing events (virtual/in-person).
+- [x] Speaking at AI/ML conferences.
+- [x] Mentoring others in PyTorch.
+- [ ] Creating technical content (e.g., blogs, videos, tutorials).
+How Would the Nominee Contribute as an Ambassador?
+```markdown
+Additional Notes:
+```markdown</t>
         </is>
       </c>
     </row>
@@ -497,10 +513,26 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>🏆 Ambassador Contribution Plan:
-🔗 Additional Information:
-✅ Contribution Highlights:
-I am **nominating someone else** to become a PyTorch Ambassador.; The nominee is **18 years of age or older**.; The nominee **agrees to abide by the [PyTorch Code of Conduct](https://github.com/pytorch-fdn/Foundation/blob/main/PyTorch%20Foundation%20Code%20of%20Conduct.md)**.; The nominee **agrees to comply with the [Linux Foundation Antitrust Policy](https://www.linuxfoundation.org/legal/antitrust-policy)**.; The nominee meets **at least one** of the qualifications listed in the [PyTorch Ambassador Program Requirements](https://github.com/pytorch-fdn/ambassador-program/blob/main/README.md).; A researcher or educator using PyTorch in academic work or training.; Organizing events (virtual/in-person).; Mentoring others in PyTorch.; Creating technical content (e.g., blogs, videos, tutorials).</t>
+          <t>Contributions:
+- [ ] I am **nominating myself** for the PyTorch Ambassador Program.
+- [x] I am **nominating someone else** to become a PyTorch Ambassador.
+- [x] The nominee is **18 years of age or older**.
+- [x] The nominee **agrees to abide by the [PyTorch Code of Conduct](https://github.com/pytorch-fdn/Foundation/blob/main/PyTorch%20Foundation%20Code%20of%20Conduct.md)**.
+- [x] The nominee **agrees to comply with the [Linux Foundation Antitrust Policy](https://www.linuxfoundation.org/legal/antitrust-policy)**.
+- [x] The nominee meets **at least one** of the qualifications listed in the [PyTorch Ambassador Program Requirements](https://github.com/pytorch-fdn/ambassador-program/blob/main/README.md).
+- [ ] An active contributor to PyTorch repositories (e.g., commits, PRs, discussions).
+- [ ] A speaker at PyTorch events or workshops.
+- [ ] A PyTorch user group organizer or meetup host.
+- [x] A researcher or educator using PyTorch in academic work or training.
+- [ ] An active leader in the PyTorch community with **at least one year** of experience in:
+- [x] Organizing events (virtual/in-person).
+- [ ] Speaking at AI/ML conferences.
+- [x] Mentoring others in PyTorch.
+- [x] Creating technical content (e.g., blogs, videos, tutorials).
+How Would the Nominee Contribute as an Ambassador?
+```markdown
+Additional Notes:
+```markdown</t>
         </is>
       </c>
     </row>
@@ -525,10 +557,26 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>🏆 Ambassador Contribution Plan:
-🔗 Additional Information:
-✅ Contribution Highlights:
-I am **nominating someone else** to become a PyTorch Ambassador.; The nominee is **18 years of age or older**.; The nominee **agrees to abide by the [PyTorch Code of Conduct](https://github.com/pytorch-fdn/Foundation/blob/main/PyTorch%20Foundation%20Code%20of%20Conduct.md)**.; The nominee **agrees to comply with the [Linux Foundation Antitrust Policy](https://www.linuxfoundation.org/legal/antitrust-policy)**.; The nominee meets **at least one** of the qualifications listed in the [PyTorch Ambassador Program Requirements](https://github.com/pytorch-fdn/ambassador-program/blob/main/README.md).; A researcher or educator using PyTorch in academic work or training.; Organizing events (virtual/in-person).; Mentoring others in PyTorch.; Creating technical content (e.g., blogs, videos, tutorials).</t>
+          <t>Contributions:
+- [ ] I am **nominating myself** for the PyTorch Ambassador Program.
+- [x] I am **nominating someone else** to become a PyTorch Ambassador.
+- [x] The nominee is **18 years of age or older**.
+- [x] The nominee **agrees to abide by the [PyTorch Code of Conduct](https://github.com/pytorch-fdn/Foundation/blob/main/PyTorch%20Foundation%20Code%20of%20Conduct.md)**.
+- [x] The nominee **agrees to comply with the [Linux Foundation Antitrust Policy](https://www.linuxfoundation.org/legal/antitrust-policy)**.
+- [x] The nominee meets **at least one** of the qualifications listed in the [PyTorch Ambassador Program Requirements](https://github.com/pytorch-fdn/ambassador-program/blob/main/README.md).
+- [ ] An active contributor to PyTorch repositories (e.g., commits, PRs, discussions).
+- [ ] A speaker at PyTorch events or workshops.
+- [ ] A PyTorch user group organizer or meetup host.
+- [x] A researcher or educator using PyTorch in academic work or training.
+- [ ] An active leader in the PyTorch community with **at least one year** of experience in:
+- [x] Organizing events (virtual/in-person).
+- [ ] Speaking at AI/ML conferences.
+- [x] Mentoring others in PyTorch.
+- [x] Creating technical content (e.g., blogs, videos, tutorials).
+How Would the Nominee Contribute as an Ambassador?
+```markdown
+Additional Notes:
+```markdown</t>
         </is>
       </c>
     </row>
@@ -553,10 +601,26 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>🏆 Ambassador Contribution Plan:
-🔗 Additional Information:
-✅ Contribution Highlights:
-I am **nominating someone else** to become a PyTorch Ambassador.; The nominee is **18 years of age or older**.; The nominee **agrees to abide by the [PyTorch Code of Conduct](https://github.com/pytorch-fdn/Foundation/blob/main/PyTorch%20Foundation%20Code%20of%20Conduct.md)**.; The nominee **agrees to comply with the [Linux Foundation Antitrust Policy](https://www.linuxfoundation.org/legal/antitrust-policy)**.; The nominee meets **at least one** of the qualifications listed in the [PyTorch Ambassador Program Requirements](https://github.com/pytorch-fdn/ambassador-program/blob/main/README.md).; An active contributor to PyTorch repositories (e.g., commits, PRs, discussions).</t>
+          <t>Contributions:
+- [ ] I am **nominating myself** for the PyTorch Ambassador Program.
+- [x] I am **nominating someone else** to become a PyTorch Ambassador.
+- [x] The nominee is **18 years of age or older**.
+- [x] The nominee **agrees to abide by the [PyTorch Code of Conduct](https://github.com/pytorch-fdn/Foundation/blob/main/PyTorch%20Foundation%20Code%20of%20Conduct.md)**.
+- [x] The nominee **agrees to comply with the [Linux Foundation Antitrust Policy](https://www.linuxfoundation.org/legal/antitrust-policy)**.
+- [x] The nominee meets **at least one** of the qualifications listed in the [PyTorch Ambassador Program Requirements](https://github.com/pytorch-fdn/ambassador-program/blob/main/README.md).
+- [x] An active contributor to PyTorch repositories (e.g., commits, PRs, discussions).
+- [ ] A speaker at PyTorch events or workshops.
+- [ ] A PyTorch user group organizer or meetup host.
+- [ ] A researcher or educator using PyTorch in academic work or training.
+- [ ] An active leader in the PyTorch community with **at least one year** of experience in:
+- [ ] Organizing events (virtual/in-person).
+- [ ] Speaking at AI/ML conferences.
+- [ ] Mentoring others in PyTorch.
+- [ ] Creating technical content (e.g., blogs, videos, tutorials).
+How Would the Nominee Contribute as an Ambassador?
+```markdown
+Additional Notes:
+```markdown</t>
         </is>
       </c>
     </row>
@@ -581,10 +645,26 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>🏆 Ambassador Contribution Plan:
-🔗 Additional Information:
-✅ Contribution Highlights:
-I am **nominating someone else** to become a PyTorch Ambassador.; The nominee is **18 years of age or older**.; The nominee **agrees to abide by the [PyTorch Code of Conduct](https://github.com/pytorch-fdn/Foundation/blob/main/PyTorch%20Foundation%20Code%20of%20Conduct.md)**.; The nominee **agrees to comply with the [Linux Foundation Antitrust Policy](https://www.linuxfoundation.org/legal/antitrust-policy)**.; The nominee meets **at least one** of the qualifications listed in the [PyTorch Ambassador Program Requirements](https://github.com/pytorch-fdn/ambassador-program/blob/main/README.md).; An active contributor to PyTorch repositories (e.g., commits, PRs, discussions).; A researcher or educator using PyTorch in academic work or training.; An active leader in the PyTorch community with **at least one year** of experience in:; Mentoring others in PyTorch.; Creating technical content (e.g., blogs, videos, tutorials).</t>
+          <t>Contributions:
+- [ ] I am **nominating myself** for the PyTorch Ambassador Program.
+- [x] I am **nominating someone else** to become a PyTorch Ambassador.
+- [x] The nominee is **18 years of age or older**.
+- [x] The nominee **agrees to abide by the [PyTorch Code of Conduct](https://github.com/pytorch-fdn/Foundation/blob/main/PyTorch%20Foundation%20Code%20of%20Conduct.md)**.
+- [x] The nominee **agrees to comply with the [Linux Foundation Antitrust Policy](https://www.linuxfoundation.org/legal/antitrust-policy)**.
+- [x] The nominee meets **at least one** of the qualifications listed in the [PyTorch Ambassador Program Requirements](https://github.com/pytorch-fdn/ambassador-program/blob/main/README.md).
+- [x] An active contributor to PyTorch repositories (e.g., commits, PRs, discussions).
+- [ ] A speaker at PyTorch events or workshops.
+- [ ] A PyTorch user group organizer or meetup host.
+- [x] A researcher or educator using PyTorch in academic work or training.
+- [x] An active leader in the PyTorch community with **at least one year** of experience in:
+- [ ] Organizing events (virtual/in-person).
+- [ ] Speaking at AI/ML conferences.
+- [x] Mentoring others in PyTorch.
+- [x] Creating technical content (e.g., blogs, videos, tutorials).
+How Would the Nominee Contribute as an Ambassador?
+```markdown
+Additional Notes:
+```markdown</t>
         </is>
       </c>
     </row>
@@ -609,10 +689,26 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>🏆 Ambassador Contribution Plan:
-🔗 Additional Information:
-✅ Contribution Highlights:
-I am **nominating someone else** to become a PyTorch Ambassador.; The nominee is **18 years of age or older**.; The nominee **agrees to abide by the [PyTorch Code of Conduct](https://github.com/pytorch-fdn/Foundation/blob/main/PyTorch%20Foundation%20Code%20of%20Conduct.md)**.; The nominee **agrees to comply with the [Linux Foundation Antitrust Policy](https://www.linuxfoundation.org/legal/antitrust-policy)**.; The nominee meets **at least one** of the qualifications listed in the [PyTorch Ambassador Program Requirements](https://github.com/pytorch-fdn/ambassador-program/blob/main/README.md).; A researcher or educator using PyTorch in academic work or training.; Organizing events (virtual/in-person).; Mentoring others in PyTorch.; Creating technical content (e.g., blogs, videos, tutorials).</t>
+          <t>Contributions:
+- [ ] I am **nominating myself** for the PyTorch Ambassador Program.
+- [x] I am **nominating someone else** to become a PyTorch Ambassador.
+- [x] The nominee is **18 years of age or older**.
+- [x] The nominee **agrees to abide by the [PyTorch Code of Conduct](https://github.com/pytorch-fdn/Foundation/blob/main/PyTorch%20Foundation%20Code%20of%20Conduct.md)**.
+- [x] The nominee **agrees to comply with the [Linux Foundation Antitrust Policy](https://www.linuxfoundation.org/legal/antitrust-policy)**.
+- [x] The nominee meets **at least one** of the qualifications listed in the [PyTorch Ambassador Program Requirements](https://github.com/pytorch-fdn/ambassador-program/blob/main/README.md).
+- [ ] An active contributor to PyTorch repositories (e.g., commits, PRs, discussions).
+- [ ] A speaker at PyTorch events or workshops.
+- [ ] A PyTorch user group organizer or meetup host.
+- [x] A researcher or educator using PyTorch in academic work or training.
+- [ ] An active leader in the PyTorch community with **at least one year** of experience in:
+- [x] Organizing events (virtual/in-person).
+- [ ] Speaking at AI/ML conferences.
+- [x] Mentoring others in PyTorch.
+- [x] Creating technical content (e.g., blogs, videos, tutorials).
+How Would the Nominee Contribute as an Ambassador?
+```markdown
+Additional Notes:
+```markdown</t>
         </is>
       </c>
     </row>
@@ -637,10 +733,26 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>🏆 Ambassador Contribution Plan:
-🔗 Additional Information:
-✅ Contribution Highlights:
-I am **nominating someone else** to become a PyTorch Ambassador.; The nominee is **18 years of age or older**.; The nominee **agrees to abide by the [PyTorch Code of Conduct](https://github.com/pytorch-fdn/Foundation/blob/main/PyTorch%20Foundation%20Code%20of%20Conduct.md)**.; The nominee **agrees to comply with the [Linux Foundation Antitrust Policy](https://www.linuxfoundation.org/legal/antitrust-policy)**.; The nominee meets **at least one** of the qualifications listed in the [PyTorch Ambassador Program Requirements](https://github.com/pytorch-fdn/ambassador-program/blob/main/README.md).; A researcher or educator using PyTorch in academic work or training.; Speaking at AI/ML conferences.; Mentoring others in PyTorch.</t>
+          <t>Contributions:
+- [ ] I am **nominating myself** for the PyTorch Ambassador Program.
+- [x] I am **nominating someone else** to become a PyTorch Ambassador.
+- [x] The nominee is **18 years of age or older**.
+- [x] The nominee **agrees to abide by the [PyTorch Code of Conduct](https://github.com/pytorch-fdn/Foundation/blob/main/PyTorch%20Foundation%20Code%20of%20Conduct.md)**.
+- [x] The nominee **agrees to comply with the [Linux Foundation Antitrust Policy](https://www.linuxfoundation.org/legal/antitrust-policy)**.
+- [x] The nominee meets **at least one** of the qualifications listed in the [PyTorch Ambassador Program Requirements](https://github.com/pytorch-fdn/ambassador-program/blob/main/README.md).
+- [ ] An active contributor to PyTorch repositories (e.g., commits, PRs, discussions).
+- [ ] A speaker at PyTorch events or workshops.
+- [ ] A PyTorch user group organizer or meetup host.
+- [x] A researcher or educator using PyTorch in academic work or training.
+- [ ] An active leader in the PyTorch community with **at least one year** of experience in:
+- [ ] Organizing events (virtual/in-person).
+- [x] Speaking at AI/ML conferences.
+- [x] Mentoring others in PyTorch.
+- [ ] Creating technical content (e.g., blogs, videos, tutorials).
+How Would the Nominee Contribute as an Ambassador?
+```markdown
+Additional Notes:
+```markdown</t>
         </is>
       </c>
     </row>
@@ -665,10 +777,26 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>🏆 Ambassador Contribution Plan:
-🔗 Additional Information:
-✅ Contribution Highlights:
-I am **nominating myself** for the PyTorch Ambassador Program.; The nominee is **18 years of age or older**.; The nominee **agrees to abide by the [PyTorch Code of Conduct](https://github.com/pytorch-fdn/Foundation/blob/main/PyTorch%20Foundation%20Code%20of%20Conduct.md)**.; The nominee **agrees to comply with the [Linux Foundation Antitrust Policy](https://www.linuxfoundation.org/legal/antitrust-policy)**.; The nominee meets **at least one** of the qualifications listed in the [PyTorch Ambassador Program Requirements](https://github.com/pytorch-fdn/ambassador-program/blob/main/README.md).; A researcher or educator using PyTorch in academic work or training.; An active leader in the PyTorch community with **at least one year** of experience in:; Organizing events (virtual/in-person).; Mentoring others in PyTorch.; Creating technical content (e.g., blogs, videos, tutorials).</t>
+          <t>Contributions:
+- [x] I am **nominating myself** for the PyTorch Ambassador Program.
+- [ ] I am **nominating someone else** to become a PyTorch Ambassador.
+- [x] The nominee is **18 years of age or older**.
+- [x] The nominee **agrees to abide by the [PyTorch Code of Conduct](https://github.com/pytorch-fdn/Foundation/blob/main/PyTorch%20Foundation%20Code%20of%20Conduct.md)**.
+- [x] The nominee **agrees to comply with the [Linux Foundation Antitrust Policy](https://www.linuxfoundation.org/legal/antitrust-policy)**.
+- [x] The nominee meets **at least one** of the qualifications listed in the [PyTorch Ambassador Program Requirements](https://github.com/pytorch-fdn/ambassador-program/blob/main/README.md).
+- [ ] An active contributor to PyTorch repositories (e.g., commits, PRs, discussions).
+- [ ] A speaker at PyTorch events or workshops.
+- [ ] A PyTorch user group organizer or meetup host.
+- [x] A researcher or educator using PyTorch in academic work or training.
+- [x] An active leader in the PyTorch community with **at least one year** of experience in:
+- [x] Organizing events (virtual/in-person).
+- [ ] Speaking at AI/ML conferences.
+- [x] Mentoring others in PyTorch.
+- [x] Creating technical content (e.g., blogs, videos, tutorials).
+How Would the Nominee Contribute as an Ambassador?
+```markdown
+Additional Notes:
+```markdown</t>
         </is>
       </c>
     </row>
@@ -693,10 +821,26 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>🏆 Ambassador Contribution Plan:
-🔗 Additional Information:
-✅ Contribution Highlights:
-I am **nominating someone else** to become a PyTorch Ambassador.; The nominee is **18 years of age or older**.; The nominee **agrees to abide by the [PyTorch Code of Conduct](https://github.com/pytorch-fdn/Foundation/blob/main/PyTorch%20Foundation%20Code%20of%20Conduct.md)**.; The nominee **agrees to comply with the [Linux Foundation Antitrust Policy](https://www.linuxfoundation.org/legal/antitrust-policy)**.; The nominee meets **at least one** of the qualifications listed in the [PyTorch Ambassador Program Requirements](https://github.com/pytorch-fdn/ambassador-program/blob/main/README.md).; A researcher or educator using PyTorch in academic work or training.; Organizing events (virtual/in-person).; Mentoring others in PyTorch.; Creating technical content (e.g., blogs, videos, tutorials).</t>
+          <t>Contributions:
+- [ ] I am **nominating myself** for the PyTorch Ambassador Program.
+- [x] I am **nominating someone else** to become a PyTorch Ambassador.
+- [x] The nominee is **18 years of age or older**.
+- [x] The nominee **agrees to abide by the [PyTorch Code of Conduct](https://github.com/pytorch-fdn/Foundation/blob/main/PyTorch%20Foundation%20Code%20of%20Conduct.md)**.
+- [x] The nominee **agrees to comply with the [Linux Foundation Antitrust Policy](https://www.linuxfoundation.org/legal/antitrust-policy)**.
+- [x] The nominee meets **at least one** of the qualifications listed in the [PyTorch Ambassador Program Requirements](https://github.com/pytorch-fdn/ambassador-program/blob/main/README.md).
+- [ ] An active contributor to PyTorch repositories (e.g., commits, PRs, discussions).
+- [ ] A speaker at PyTorch events or workshops.
+- [ ] A PyTorch user group organizer or meetup host.
+- [x] A researcher or educator using PyTorch in academic work or training.
+- [ ] An active leader in the PyTorch community with **at least one year** of experience in:
+- [x] Organizing events (virtual/in-person).
+- [ ] Speaking at AI/ML conferences.
+- [x] Mentoring others in PyTorch.
+- [x] Creating technical content (e.g., blogs, videos, tutorials).
+How Would the Nominee Contribute as an Ambassador?
+```markdown
+Additional Notes:
+```markdown</t>
         </is>
       </c>
     </row>
@@ -721,10 +865,26 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>🏆 Ambassador Contribution Plan:
-🔗 Additional Information:
-✅ Contribution Highlights:
-I am **nominating someone else** to become a PyTorch Ambassador.; The nominee is **18 years of age or older**.; The nominee **agrees to abide by the [PyTorch Code of Conduct](https://github.com/pytorch-fdn/Foundation/blob/main/PyTorch%20Foundation%20Code%20of%20Conduct.md)**.; The nominee **agrees to comply with the [Linux Foundation Antitrust Policy](https://www.linuxfoundation.org/legal/antitrust-policy)**.; The nominee meets **at least one** of the qualifications listed in the [PyTorch Ambassador Program Requirements](https://github.com/pytorch-fdn/ambassador-program/blob/main/README.md).; A researcher or educator using PyTorch in academic work or training.; Organizing events (virtual/in-person).; Mentoring others in PyTorch.; Creating technical content (e.g., blogs, videos, tutorials).</t>
+          <t>Contributions:
+- [ ] I am **nominating myself** for the PyTorch Ambassador Program.
+- [x] I am **nominating someone else** to become a PyTorch Ambassador.
+- [x] The nominee is **18 years of age or older**.
+- [x] The nominee **agrees to abide by the [PyTorch Code of Conduct](https://github.com/pytorch-fdn/Foundation/blob/main/PyTorch%20Foundation%20Code%20of%20Conduct.md)**.
+- [x] The nominee **agrees to comply with the [Linux Foundation Antitrust Policy](https://www.linuxfoundation.org/legal/antitrust-policy)**.
+- [x] The nominee meets **at least one** of the qualifications listed in the [PyTorch Ambassador Program Requirements](https://github.com/pytorch-fdn/ambassador-program/blob/main/README.md).
+- [ ] An active contributor to PyTorch repositories (e.g., commits, PRs, discussions).
+- [ ] A speaker at PyTorch events or workshops.
+- [ ] A PyTorch user group organizer or meetup host.
+- [x] A researcher or educator using PyTorch in academic work or training.
+- [ ] An active leader in the PyTorch community with **at least one year** of experience in:
+- [x] Organizing events (virtual/in-person).
+- [ ] Speaking at AI/ML conferences.
+- [x] Mentoring others in PyTorch.
+- [x] Creating technical content (e.g., blogs, videos, tutorials).
+How Would the Nominee Contribute as an Ambassador?
+```markdown
+Additional Notes:
+```markdown</t>
         </is>
       </c>
     </row>
@@ -749,10 +909,26 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>🏆 Ambassador Contribution Plan:
-🔗 Additional Information:
-✅ Contribution Highlights:
-I am **nominating someone else** to become a PyTorch Ambassador.; The nominee is **18 years of age or older**.; The nominee **agrees to abide by the [PyTorch Code of Conduct](https://github.com/pytorch-fdn/Foundation/blob/main/PyTorch%20Foundation%20Code%20of%20Conduct.md)**.; The nominee **agrees to comply with the [Linux Foundation Antitrust Policy](https://www.linuxfoundation.org/legal/antitrust-policy)**.; The nominee meets **at least one** of the qualifications listed in the [PyTorch Ambassador Program Requirements](https://github.com/pytorch-fdn/ambassador-program/blob/main/README.md).; A researcher or educator using PyTorch in academic work or training.; Organizing events (virtual/in-person).; Speaking at AI/ML conferences.; Creating technical content (e.g., blogs, videos, tutorials).</t>
+          <t>Contributions:
+- [ ] I am **nominating myself** for the PyTorch Ambassador Program.
+- [x] I am **nominating someone else** to become a PyTorch Ambassador.
+- [x] The nominee is **18 years of age or older**.
+- [x] The nominee **agrees to abide by the [PyTorch Code of Conduct](https://github.com/pytorch-fdn/Foundation/blob/main/PyTorch%20Foundation%20Code%20of%20Conduct.md)**.
+- [x] The nominee **agrees to comply with the [Linux Foundation Antitrust Policy](https://www.linuxfoundation.org/legal/antitrust-policy)**.
+- [x] The nominee meets **at least one** of the qualifications listed in the [PyTorch Ambassador Program Requirements](https://github.com/pytorch-fdn/ambassador-program/blob/main/README.md).
+- [ ] An active contributor to PyTorch repositories (e.g., commits, PRs, discussions).
+- [ ] A speaker at PyTorch events or workshops.
+- [ ] A PyTorch user group organizer or meetup host.
+- [x] A researcher or educator using PyTorch in academic work or training.
+- [ ] An active leader in the PyTorch community with **at least one year** of experience in:
+- [x] Organizing events (virtual/in-person).
+- [x] Speaking at AI/ML conferences.
+- [ ] Mentoring others in PyTorch.
+- [x] Creating technical content (e.g., blogs, videos, tutorials).
+How Would the Nominee Contribute as an Ambassador?
+```markdown
+Additional Notes:
+```markdown</t>
         </is>
       </c>
     </row>
@@ -777,10 +953,26 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>🏆 Ambassador Contribution Plan:
-🔗 Additional Information:
-✅ Contribution Highlights:
-I am **nominating myself** for the PyTorch Ambassador Program.; The nominee is **18 years of age or older**.; The nominee **agrees to abide by the [PyTorch Code of Conduct](https://github.com/pytorch-fdn/Foundation/blob/main/PyTorch%20Foundation%20Code%20of%20Conduct.md)**.; The nominee **agrees to comply with the [Linux Foundation Antitrust Policy](https://www.linuxfoundation.org/legal/antitrust-policy)**.; The nominee meets **at least one** of the qualifications listed in the [PyTorch Ambassador Program Requirements](https://github.com/pytorch-fdn/ambassador-program/blob/main/README.md).; A researcher or educator using PyTorch in academic work or training.; Organizing events (virtual/in-person).; Speaking at AI/ML conferences.; Creating technical content (e.g., blogs, videos, tutorials).</t>
+          <t>Contributions:
+- [x] I am **nominating myself** for the PyTorch Ambassador Program.
+- [ ] I am **nominating someone else** to become a PyTorch Ambassador.
+- [x] The nominee is **18 years of age or older**.
+- [x] The nominee **agrees to abide by the [PyTorch Code of Conduct](https://github.com/pytorch-fdn/Foundation/blob/main/PyTorch%20Foundation%20Code%20of%20Conduct.md)**.
+- [x] The nominee **agrees to comply with the [Linux Foundation Antitrust Policy](https://www.linuxfoundation.org/legal/antitrust-policy)**.
+- [x] The nominee meets **at least one** of the qualifications listed in the [PyTorch Ambassador Program Requirements](https://github.com/pytorch-fdn/ambassador-program/blob/main/README.md).
+- [ ] An active contributor to PyTorch repositories (e.g., commits, PRs, discussions).
+- [ ] A speaker at PyTorch events or workshops.
+- [ ] A PyTorch user group organizer or meetup host.
+- [x] A researcher or educator using PyTorch in academic work or training.
+- [ ] An active leader in the PyTorch community with **at least one year** of experience in:
+- [x] Organizing events (virtual/in-person).
+- [x] Speaking at AI/ML conferences.
+- [ ] Mentoring others in PyTorch.
+- [x] Creating technical content (e.g., blogs, videos, tutorials).
+How Would the Nominee Contribute as an Ambassador?
+```markdown
+Additional Notes:
+```markdown</t>
         </is>
       </c>
     </row>
@@ -805,10 +997,26 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>🏆 Ambassador Contribution Plan:
-🔗 Additional Information:
-✅ Contribution Highlights:
-I am **nominating myself** for the PyTorch Ambassador Program.; The nominee is **18 years of age or older**.; The nominee **agrees to abide by the [PyTorch Code of Conduct](https://github.com/pytorch-fdn/Foundation/blob/main/PyTorch%20Foundation%20Code%20of%20Conduct.md)**.; The nominee **agrees to comply with the [Linux Foundation Antitrust Policy](https://www.linuxfoundation.org/legal/antitrust-policy)**.; The nominee meets **at least one** of the qualifications listed in the [PyTorch Ambassador Program Requirements](https://github.com/pytorch-fdn/ambassador-program/blob/main/README.md).; An active contributor to PyTorch repositories (e.g., commits, PRs, discussions).; A researcher or educator using PyTorch in academic work or training.; Organizing events (virtual/in-person).; Mentoring others in PyTorch.; Creating technical content (e.g., blogs, videos, tutorials).</t>
+          <t>Contributions:
+- [x] I am **nominating myself** for the PyTorch Ambassador Program.
+- [ ] I am **nominating someone else** to become a PyTorch Ambassador.
+- [x] The nominee is **18 years of age or older**.
+- [x] The nominee **agrees to abide by the [PyTorch Code of Conduct](https://github.com/pytorch-fdn/Foundation/blob/main/PyTorch%20Foundation%20Code%20of%20Conduct.md)**.
+- [x] The nominee **agrees to comply with the [Linux Foundation Antitrust Policy](https://www.linuxfoundation.org/legal/antitrust-policy)**.
+- [x] The nominee meets **at least one** of the qualifications listed in the [PyTorch Ambassador Program Requirements](https://github.com/pytorch-fdn/ambassador-program/blob/main/README.md).
+- [x] An active contributor to PyTorch repositories (e.g., commits, PRs, discussions).
+- [ ] A speaker at PyTorch events or workshops.
+- [ ] A PyTorch user group organizer or meetup host.
+- [x] A researcher or educator using PyTorch in academic work or training.
+- [ ] An active leader in the PyTorch community with **at least one year** of experience in:
+- [x] Organizing events (virtual/in-person).
+- [ ] Speaking at AI/ML conferences.
+- [x] Mentoring others in PyTorch.
+- [x] Creating technical content (e.g., blogs, videos, tutorials).
+How Would the Nominee Contribute as an Ambassador?
+```markdown
+Additional Notes:
+```markdown</t>
         </is>
       </c>
     </row>
@@ -833,10 +1041,26 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>🏆 Ambassador Contribution Plan:
-🔗 Additional Information:
-✅ Contribution Highlights:
-I am **nominating myself** for the PyTorch Ambassador Program.; The nominee **agrees to abide by the [PyTorch Code of Conduct](https://github.com/pytorch-fdn/Foundation/blob/main/PyTorch%20Foundation%20Code%20of%20Conduct.md)**.; The nominee **agrees to comply with the [Linux Foundation Antitrust Policy](https://www.linuxfoundation.org/legal/antitrust-policy)**.; The nominee meets **at least one** of the qualifications listed in the [PyTorch Ambassador Program Requirements](https://github.com/pytorch-fdn/ambassador-program/blob/main/README.md).; A researcher or educator using PyTorch in academic work or training.; An active leader in the PyTorch community with **at least one year** of experience in:; Organizing events (virtual/in-person).; Speaking at AI/ML conferences.; Mentoring others in PyTorch.; Creating technical content (e.g., blogs, videos, tutorials).</t>
+          <t>Contributions:
+- [x] I am **nominating myself** for the PyTorch Ambassador Program.
+- [ ] I am **nominating someone else** to become a PyTorch Ambassador.
+- [ ] The nominee is **18 years of age or older**.
+- [x] The nominee **agrees to abide by the [PyTorch Code of Conduct](https://github.com/pytorch-fdn/Foundation/blob/main/PyTorch%20Foundation%20Code%20of%20Conduct.md)**.
+- [x] The nominee **agrees to comply with the [Linux Foundation Antitrust Policy](https://www.linuxfoundation.org/legal/antitrust-policy)**.
+- [x] The nominee meets **at least one** of the qualifications listed in the [PyTorch Ambassador Program Requirements](https://github.com/pytorch-fdn/ambassador-program/blob/main/README.md).
+- [ ] An active contributor to PyTorch repositories (e.g., commits, PRs, discussions).
+- [ ] A speaker at PyTorch events or workshops.
+- [ ] A PyTorch user group organizer or meetup host.
+- [x] A researcher or educator using PyTorch in academic work or training.
+- [x] An active leader in the PyTorch community with **at least one year** of experience in:
+- [x] Organizing events (virtual/in-person).
+- [x] Speaking at AI/ML conferences.
+- [x] Mentoring others in PyTorch.
+- [x] Creating technical content (e.g., blogs, videos, tutorials).
+How Would the Nominee Contribute as an Ambassador?
+```markdown
+Additional Notes:
+```markdown</t>
         </is>
       </c>
     </row>
@@ -861,10 +1085,26 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>🏆 Ambassador Contribution Plan:
-🔗 Additional Information:
-✅ Contribution Highlights:
-I am **nominating myself** for the PyTorch Ambassador Program.; The nominee is **18 years of age or older**.; The nominee **agrees to abide by the [PyTorch Code of Conduct](https://github.com/pytorch-fdn/Foundation/blob/main/PyTorch%20Foundation%20Code%20of%20Conduct.md)**.; The nominee **agrees to comply with the [Linux Foundation Antitrust Policy](https://www.linuxfoundation.org/legal/antitrust-policy)**.; The nominee meets **at least one** of the qualifications listed in the [PyTorch Ambassador Program Requirements](https://github.com/pytorch-fdn/ambassador-program/blob/main/README.md).; Organizing events (virtual/in-person).; Speaking at AI/ML conferences.; Creating technical content (e.g., blogs, videos, tutorials).</t>
+          <t>Contributions:
+- [x] I am **nominating myself** for the PyTorch Ambassador Program.
+- [ ] I am **nominating someone else** to become a PyTorch Ambassador.
+- [x] The nominee is **18 years of age or older**.
+- [x] The nominee **agrees to abide by the [PyTorch Code of Conduct](https://github.com/pytorch-fdn/Foundation/blob/main/PyTorch%20Foundation%20Code%20of%20Conduct.md)**.
+- [x] The nominee **agrees to comply with the [Linux Foundation Antitrust Policy](https://www.linuxfoundation.org/legal/antitrust-policy)**.
+- [x] The nominee meets **at least one** of the qualifications listed in the [PyTorch Ambassador Program Requirements](https://github.com/pytorch-fdn/ambassador-program/blob/main/README.md).
+- [ ] An active contributor to PyTorch repositories (e.g., commits, PRs, discussions).
+- [ ] A speaker at PyTorch events or workshops.
+- [ ] A PyTorch user group organizer or meetup host.
+- [ ] A researcher or educator using PyTorch in academic work or training.
+- [ ] An active leader in the PyTorch community with **at least one year** of experience in:
+- [x] Organizing events (virtual/in-person).
+- [x] Speaking at AI/ML conferences.
+- [ ] Mentoring others in PyTorch.
+- [x] Creating technical content (e.g., blogs, videos, tutorials).
+How Would the Nominee Contribute as an Ambassador?
+```markdown
+Additional Notes:
+```markdown</t>
         </is>
       </c>
     </row>
@@ -889,10 +1129,26 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>🏆 Ambassador Contribution Plan:
-🔗 Additional Information:
-✅ Contribution Highlights:
-I am **nominating myself** for the PyTorch Ambassador Program.; The nominee is **18 years of age or older**.; The nominee **agrees to abide by the [PyTorch Code of Conduct](https://github.com/pytorch-fdn/Foundation/blob/main/PyTorch%20Foundation%20Code%20of%20Conduct.md)**.; The nominee **agrees to comply with the [Linux Foundation Antitrust Policy](https://www.linuxfoundation.org/legal/antitrust-policy)**.; The nominee meets **at least one** of the qualifications listed in the [PyTorch Ambassador Program Requirements](https://github.com/pytorch-fdn/ambassador-program/blob/main/README.md).; Organizing events (virtual/in-person).; Speaking at AI/ML conferences.; Creating technical content (e.g., blogs, videos, tutorials).</t>
+          <t>Contributions:
+- [x] I am **nominating myself** for the PyTorch Ambassador Program.
+- [ ] I am **nominating someone else** to become a PyTorch Ambassador.
+- [x] The nominee is **18 years of age or older**.
+- [x] The nominee **agrees to abide by the [PyTorch Code of Conduct](https://github.com/pytorch-fdn/Foundation/blob/main/PyTorch%20Foundation%20Code%20of%20Conduct.md)**.
+- [x] The nominee **agrees to comply with the [Linux Foundation Antitrust Policy](https://www.linuxfoundation.org/legal/antitrust-policy)**.
+- [x] The nominee meets **at least one** of the qualifications listed in the [PyTorch Ambassador Program Requirements](https://github.com/pytorch-fdn/ambassador-program/blob/main/README.md).
+- [ ] An active contributor to PyTorch repositories (e.g., commits, PRs, discussions).
+- [ ] A speaker at PyTorch events or workshops.
+- [ ] A PyTorch user group organizer or meetup host.
+- [ ] A researcher or educator using PyTorch in academic work or training.
+- [ ] An active leader in the PyTorch community with **at least one year** of experience in:
+- [x] Organizing events (virtual/in-person).
+- [x] Speaking at AI/ML conferences.
+- [ ] Mentoring others in PyTorch.
+- [x] Creating technical content (e.g., blogs, videos, tutorials).
+How Would the Nominee Contribute as an Ambassador?
+```markdown
+Additional Notes:
+```markdown</t>
         </is>
       </c>
     </row>
@@ -917,10 +1173,26 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>🏆 Ambassador Contribution Plan:
-🔗 Additional Information:
-✅ Contribution Highlights:
-I am **nominating myself** for the PyTorch Ambassador Program.; The nominee is **18 years of age or older**.; The nominee **agrees to abide by the [PyTorch Code of Conduct](https://github.com/pytorch-fdn/Foundation/blob/main/PyTorch%20Foundation%20Code%20of%20Conduct.md)**.; The nominee **agrees to comply with the [Linux Foundation Antitrust Policy](https://www.linuxfoundation.org/legal/antitrust-policy)**.; The nominee meets **at least one** of the qualifications listed in the [PyTorch Ambassador Program Requirements](https://github.com/pytorch-fdn/ambassador-program/blob/main/README.md).; An active contributor to PyTorch repositories (e.g., commits, PRs, discussions).; A researcher or educator using PyTorch in academic work or training.; Speaking at AI/ML conferences.; Mentoring others in PyTorch.; Creating technical content (e.g., blogs, videos, tutorials).</t>
+          <t>Contributions:
+- [x] I am **nominating myself** for the PyTorch Ambassador Program.
+- [ ] I am **nominating someone else** to become a PyTorch Ambassador.
+- [x] The nominee is **18 years of age or older**.
+- [x] The nominee **agrees to abide by the [PyTorch Code of Conduct](https://github.com/pytorch-fdn/Foundation/blob/main/PyTorch%20Foundation%20Code%20of%20Conduct.md)**.
+- [x] The nominee **agrees to comply with the [Linux Foundation Antitrust Policy](https://www.linuxfoundation.org/legal/antitrust-policy)**.
+- [x] The nominee meets **at least one** of the qualifications listed in the [PyTorch Ambassador Program Requirements](https://github.com/pytorch-fdn/ambassador-program/blob/main/README.md).
+- [x] An active contributor to PyTorch repositories (e.g., commits, PRs, discussions).
+- [ ] A speaker at PyTorch events or workshops.
+- [ ] A PyTorch user group organizer or meetup host.
+- [x] A researcher or educator using PyTorch in academic work or training.
+- [ ] An active leader in the PyTorch community with **at least one year** of experience in:
+- [ ] Organizing events (virtual/in-person).
+- [x] Speaking at AI/ML conferences.
+- [x] Mentoring others in PyTorch.
+- [x] Creating technical content (e.g., blogs, videos, tutorials).
+How Would the Nominee Contribute as an Ambassador?
+```markdown
+Additional Notes:
+```markdown</t>
         </is>
       </c>
     </row>
@@ -945,10 +1217,26 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>🏆 Ambassador Contribution Plan:
-🔗 Additional Information:
-✅ Contribution Highlights:
-I am **nominating myself** for the PyTorch Ambassador Program.; The nominee is **18 years of age or older**.; The nominee **agrees to abide by the [PyTorch Code of Conduct](https://github.com/pytorch-fdn/Foundation/blob/main/PyTorch%20Foundation%20Code%20of%20Conduct.md)**.; The nominee **agrees to comply with the [Linux Foundation Antitrust Policy](https://www.linuxfoundation.org/legal/antitrust-policy)**.; The nominee meets **at least one** of the qualifications listed in the [PyTorch Ambassador Program Requirements](https://github.com/pytorch-fdn/ambassador-program/blob/main/README.md).; An active contributor to PyTorch repositories (e.g., commits, PRs, discussions).; A researcher or educator using PyTorch in academic work or training.; Speaking at AI/ML conferences.; Mentoring others in PyTorch.; Creating technical content (e.g., blogs, videos, tutorials).</t>
+          <t>Contributions:
+- [x] I am **nominating myself** for the PyTorch Ambassador Program.
+- [ ] I am **nominating someone else** to become a PyTorch Ambassador.
+- [x] The nominee is **18 years of age or older**.
+- [x] The nominee **agrees to abide by the [PyTorch Code of Conduct](https://github.com/pytorch-fdn/Foundation/blob/main/PyTorch%20Foundation%20Code%20of%20Conduct.md)**.
+- [x] The nominee **agrees to comply with the [Linux Foundation Antitrust Policy](https://www.linuxfoundation.org/legal/antitrust-policy)**.
+- [x] The nominee meets **at least one** of the qualifications listed in the [PyTorch Ambassador Program Requirements](https://github.com/pytorch-fdn/ambassador-program/blob/main/README.md).
+- [x] An active contributor to PyTorch repositories (e.g., commits, PRs, discussions).
+- [ ] A speaker at PyTorch events or workshops.
+- [ ] A PyTorch user group organizer or meetup host.
+- [x] A researcher or educator using PyTorch in academic work or training.
+- [ ] An active leader in the PyTorch community with **at least one year** of experience in:
+- [ ] Organizing events (virtual/in-person).
+- [x] Speaking at AI/ML conferences.
+- [x] Mentoring others in PyTorch.
+- [x] Creating technical content (e.g., blogs, videos, tutorials).
+How Would the Nominee Contribute as an Ambassador?
+```markdown
+Additional Notes:
+```markdown</t>
         </is>
       </c>
     </row>
@@ -973,10 +1261,26 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>🏆 Ambassador Contribution Plan:
-🔗 Additional Information:
-✅ Contribution Highlights:
-I am **nominating someone else** to become a PyTorch Ambassador.; The nominee is **18 years of age or older**.; The nominee **agrees to abide by the [PyTorch Code of Conduct](https://github.com/pytorch-fdn/Foundation/blob/main/PyTorch%20Foundation%20Code%20of%20Conduct.md)**.; The nominee **agrees to comply with the [Linux Foundation Antitrust Policy](https://www.linuxfoundation.org/legal/antitrust-policy)**.; The nominee meets **at least one** of the qualifications listed in the [PyTorch Ambassador Program Requirements](https://github.com/pytorch-fdn/foundation-programs/blob/main/pytorch-ambassador-program.md).; A speaker at PyTorch events or workshops.; Speaking at AI/ML conferences.; Mentoring others in PyTorch.; Creating technical content (e.g., blogs, videos, tutorials).</t>
+          <t>Contributions:
+- [ ] I am **nominating myself** for the PyTorch Ambassador Program.
+- [x] I am **nominating someone else** to become a PyTorch Ambassador.
+- [x] The nominee is **18 years of age or older**.
+- [x] The nominee **agrees to abide by the [PyTorch Code of Conduct](https://github.com/pytorch-fdn/Foundation/blob/main/PyTorch%20Foundation%20Code%20of%20Conduct.md)**.
+- [x] The nominee **agrees to comply with the [Linux Foundation Antitrust Policy](https://www.linuxfoundation.org/legal/antitrust-policy)**.
+- [x] The nominee meets **at least one** of the qualifications listed in the [PyTorch Ambassador Program Requirements](https://github.com/pytorch-fdn/foundation-programs/blob/main/pytorch-ambassador-program.md).
+- [ ] An active contributor to PyTorch repositories (e.g., commits, PRs, discussions).
+- [x] A speaker at PyTorch events or workshops.
+- [ ] A PyTorch user group organizer or meetup host.
+- [ ] A researcher or educator using PyTorch in academic work or training.
+- [ ] An active leader in the PyTorch community with **at least one year** of experience in:
+- [ ] Organizing events (virtual/in-person).
+- [x] Speaking at AI/ML conferences.
+- [x] Mentoring others in PyTorch.
+- [x] Creating technical content (e.g., blogs, videos, tutorials).
+How Would the Nominee Contribute as an Ambassador?
+```markdown
+Additional Notes:
+```markdown</t>
         </is>
       </c>
     </row>
@@ -1001,10 +1305,26 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>🏆 Ambassador Contribution Plan:
-🔗 Additional Information:
-✅ Contribution Highlights:
-I am **nominating myself** for the PyTorch Ambassador Program.; The nominee is **18 years of age or older**.; The nominee **agrees to abide by the [PyTorch Code of Conduct](https://github.com/pytorch-fdn/Foundation/blob/main/PyTorch%20Foundation%20Code%20of%20Conduct.md)**.; The nominee **agrees to comply with the [Linux Foundation Antitrust Policy](https://www.linuxfoundation.org/legal/antitrust-policy)**.; The nominee meets **at least one** of the qualifications listed in the [PyTorch Ambassador Program Requirements](https://github.com/pytorch-fdn/foundation-programs/blob/main/pytorch-ambassador-program.md).; A speaker at PyTorch events or workshops.; A PyTorch user group organizer or meetup host.; A researcher or educator using PyTorch in academic work or training.; An active leader in the PyTorch community with **at least one year** of experience in:; Organizing events (virtual/in-person).; Speaking at AI/ML conferences.; Mentoring others in PyTorch.; Creating technical content (e.g., blogs, videos, tutorials).</t>
+          <t>Contributions:
+- [x] I am **nominating myself** for the PyTorch Ambassador Program.
+- [ ] I am **nominating someone else** to become a PyTorch Ambassador.
+- [x] The nominee is **18 years of age or older**.
+- [x] The nominee **agrees to abide by the [PyTorch Code of Conduct](https://github.com/pytorch-fdn/Foundation/blob/main/PyTorch%20Foundation%20Code%20of%20Conduct.md)**.
+- [x] The nominee **agrees to comply with the [Linux Foundation Antitrust Policy](https://www.linuxfoundation.org/legal/antitrust-policy)**.
+- [x] The nominee meets **at least one** of the qualifications listed in the [PyTorch Ambassador Program Requirements](https://github.com/pytorch-fdn/foundation-programs/blob/main/pytorch-ambassador-program.md).
+- [ ] An active contributor to PyTorch repositories (e.g., commits, PRs, discussions).
+- [x] A speaker at PyTorch events or workshops.
+- [x] A PyTorch user group organizer or meetup host.
+- [x] A researcher or educator using PyTorch in academic work or training.
+- [x] An active leader in the PyTorch community with **at least one year** of experience in:
+- [x] Organizing events (virtual/in-person).
+- [x] Speaking at AI/ML conferences.
+- [x] Mentoring others in PyTorch.
+- [x] Creating technical content (e.g., blogs, videos, tutorials).
+How Would the Nominee Contribute as an Ambassador?
+```markdown
+Additional Notes:
+```markdown</t>
         </is>
       </c>
     </row>
@@ -1029,10 +1349,26 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>🏆 Ambassador Contribution Plan:
-🔗 Additional Information:
-✅ Contribution Highlights:
-I am **nominating myself** for the PyTorch Ambassador Program.; I am **nominating someone else** to become a PyTorch Ambassador.; The nominee is **18 years of age or older**.; The nominee **agrees to abide by the [PyTorch Code of Conduct](https://github.com/pytorch-fdn/Foundation/blob/main/PyTorch%20Foundation%20Code%20of%20Conduct.md)**.; The nominee **agrees to comply with the [Linux Foundation Antitrust Policy](https://www.linuxfoundation.org/legal/antitrust-policy)**.; The nominee meets **at least one** of the qualifications listed in the [PyTorch Ambassador Program Requirements](https://github.com/pytorch-fdn/foundation-programs/blob/main/pytorch-ambassador-program.md).; A researcher or educator using PyTorch in academic work or training.; Creating technical content (e.g., blogs, videos, tutorials).</t>
+          <t>Contributions:
+- [x] I am **nominating myself** for the PyTorch Ambassador Program.
+- [x] I am **nominating someone else** to become a PyTorch Ambassador.
+- [x] The nominee is **18 years of age or older**.
+- [x] The nominee **agrees to abide by the [PyTorch Code of Conduct](https://github.com/pytorch-fdn/Foundation/blob/main/PyTorch%20Foundation%20Code%20of%20Conduct.md)**.
+- [x] The nominee **agrees to comply with the [Linux Foundation Antitrust Policy](https://www.linuxfoundation.org/legal/antitrust-policy)**.
+- [x] The nominee meets **at least one** of the qualifications listed in the [PyTorch Ambassador Program Requirements](https://github.com/pytorch-fdn/foundation-programs/blob/main/pytorch-ambassador-program.md).
+- [ ] An active contributor to PyTorch repositories (e.g., commits, PRs, discussions).
+- [ ] A speaker at PyTorch events or workshops.
+- [ ] A PyTorch user group organizer or meetup host.
+- [x] A researcher or educator using PyTorch in academic work or training.
+- [ ] An active leader in the PyTorch community with **at least one year** of experience in:
+- [ ] Organizing events (virtual/in-person).
+- [ ] Speaking at AI/ML conferences.
+- [ ] Mentoring others in PyTorch.
+- [x] Creating technical content (e.g., blogs, videos, tutorials).
+How Would the Nominee Contribute as an Ambassador?
+```markdown
+Additional Notes:
+```markdown</t>
         </is>
       </c>
     </row>
@@ -1057,10 +1393,26 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>🏆 Ambassador Contribution Plan:
-🔗 Additional Information:
-✅ Contribution Highlights:
-I am **nominating myself** for the PyTorch Ambassador Program.; The nominee is **18 years of age or older**.; The nominee **agrees to abide by the [PyTorch Code of Conduct](https://github.com/pytorch-fdn/Foundation/blob/main/PyTorch%20Foundation%20Code%20of%20Conduct.md)**.; The nominee **agrees to comply with the [Linux Foundation Antitrust Policy](https://www.linuxfoundation.org/legal/antitrust-policy)**.; The nominee meets **at least one** of the qualifications listed in the [PyTorch Ambassador Program Requirements](https://github.com/pytorch-fdn/foundation-programs/blob/main/pytorch-ambassador-program.md).; An active contributor to PyTorch repositories (e.g., commits, PRs, discussions).; Creating technical content (e.g., blogs, videos, tutorials).</t>
+          <t>Contributions:
+- [x] I am **nominating myself** for the PyTorch Ambassador Program.
+- [ ] I am **nominating someone else** to become a PyTorch Ambassador.
+- [x] The nominee is **18 years of age or older**.
+- [x] The nominee **agrees to abide by the [PyTorch Code of Conduct](https://github.com/pytorch-fdn/Foundation/blob/main/PyTorch%20Foundation%20Code%20of%20Conduct.md)**.
+- [x] The nominee **agrees to comply with the [Linux Foundation Antitrust Policy](https://www.linuxfoundation.org/legal/antitrust-policy)**.
+- [x] The nominee meets **at least one** of the qualifications listed in the [PyTorch Ambassador Program Requirements](https://github.com/pytorch-fdn/foundation-programs/blob/main/pytorch-ambassador-program.md).
+- [x] An active contributor to PyTorch repositories (e.g., commits, PRs, discussions).
+- [ ] A speaker at PyTorch events or workshops.
+- [ ] A PyTorch user group organizer or meetup host.
+- [ ] A researcher or educator using PyTorch in academic work or training.
+- [ ] An active leader in the PyTorch community with **at least one year** of experience in:
+- [ ] Organizing events (virtual/in-person).
+- [ ] Speaking at AI/ML conferences.
+- [ ] Mentoring others in PyTorch.
+- [x] Creating technical content (e.g., blogs, videos, tutorials).
+How Would the Nominee Contribute as an Ambassador?
+```markdown
+Additional Notes:
+```markdown</t>
         </is>
       </c>
     </row>
@@ -1085,10 +1437,26 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>🏆 Ambassador Contribution Plan:
-🔗 Additional Information:
-✅ Contribution Highlights:
-I am **nominating myself** for the PyTorch Ambassador Program.; The nominee is **18 years of age or older**.; The nominee **agrees to abide by the [PyTorch Code of Conduct](https://github.com/pytorch-fdn/Foundation/blob/main/PyTorch%20Foundation%20Code%20of%20Conduct.md)**.; The nominee **agrees to comply with the [Linux Foundation Antitrust Policy](https://www.linuxfoundation.org/legal/antitrust-policy)**.; The nominee meets **at least one** of the qualifications listed in the [PyTorch Ambassador Program Requirements](https://github.com/pytorch-fdn/foundation-programs/blob/main/pytorch-ambassador-program.md).; Mentoring others in PyTorch.; Creating technical content (e.g., blogs, videos, tutorials).</t>
+          <t>Contributions:
+- [x] I am **nominating myself** for the PyTorch Ambassador Program.
+- [ ] I am **nominating someone else** to become a PyTorch Ambassador.
+- [x] The nominee is **18 years of age or older**.
+- [x] The nominee **agrees to abide by the [PyTorch Code of Conduct](https://github.com/pytorch-fdn/Foundation/blob/main/PyTorch%20Foundation%20Code%20of%20Conduct.md)**.
+- [x] The nominee **agrees to comply with the [Linux Foundation Antitrust Policy](https://www.linuxfoundation.org/legal/antitrust-policy)**.
+- [x] The nominee meets **at least one** of the qualifications listed in the [PyTorch Ambassador Program Requirements](https://github.com/pytorch-fdn/foundation-programs/blob/main/pytorch-ambassador-program.md).
+- [ ] An active contributor to PyTorch repositories (e.g., commits, PRs, discussions).
+- [ ] A speaker at PyTorch events or workshops.
+- [ ] A PyTorch user group organizer or meetup host.
+- [ ] A researcher or educator using PyTorch in academic work or training.
+- [ ] An active leader in the PyTorch community with **at least one year** of experience in:
+- [ ] Organizing events (virtual/in-person).
+- [ ] Speaking at AI/ML conferences.
+- [x] Mentoring others in PyTorch.
+- [x] Creating technical content (e.g., blogs, videos, tutorials).
+How Would the Nominee Contribute as an Ambassador?
+```markdown
+Additional Notes:
+```markdown</t>
         </is>
       </c>
     </row>

</xml_diff>